<commit_message>
Add progress bar for URL processing in main.py using tqdm; handle keyboard interrupts gracefully and log partial results. Update dependencies in pyproject.toml and uv.lock to include tqdm.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles.xlsx
+++ b/output/extracted_profiles.xlsx
@@ -596,24 +596,24 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/savanah-nunes</t>
+          <t>https://www.uidaho.edu/cals/people/madison-mcguire</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Savanah</t>
+          <t>Madison</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Nunes</t>
+          <t>McGuire</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Media and Communications Manager</t>
+          <t>Administrative Specialist</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -627,24 +627,24 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/steve-greene</t>
+          <t>https://www.uidaho.edu/cals/people/savanah-nunes</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Steve</t>
+          <t>Savanah</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Greene</t>
+          <t>Nunes</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Program Manager</t>
+          <t>Media and Communications Manager</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
@@ -658,24 +658,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/amy-calabretta</t>
+          <t>https://www.uidaho.edu/cals/people/steve-greene</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Amy</t>
+          <t>Steve</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Calabretta</t>
+          <t>Greene</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Interim Director of Communications &amp; Strategic Initiatives</t>
+          <t>Program Manager</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
@@ -689,30 +689,30 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/angela-harley</t>
+          <t>https://www.uidaho.edu/cals/people/amy-calabretta</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Angela</t>
+          <t>Amy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Harley</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>Calabretta</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Interim Director of Communications &amp; Strategic Initiatives</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>College of Agricultural &amp; Life Sciences</t>
-        </is>
-      </c>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
@@ -720,30 +720,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/brandi-chastain</t>
+          <t>https://www.uidaho.edu/cals/people/angela-harley</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Brandi</t>
+          <t>Angela</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Chastain</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Management Assistant</t>
-        </is>
-      </c>
+          <t>Harley</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
@@ -751,24 +751,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/brian-kelly</t>
+          <t>https://www.uidaho.edu/cals/people/ann-barrington</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Ann</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Barrington</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>UI Extension Web Coordinator</t>
+          <t>Senior Director of Development</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
@@ -782,24 +782,24 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/carly-schoepflin</t>
+          <t>https://www.uidaho.edu/cals/people/ashley-baker</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Carly</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Schoepflin</t>
+          <t>Baker</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Director of Communications &amp; Strategic Initiatives</t>
+          <t>Instructional Media Designer</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>

</xml_diff>

<commit_message>
Enhance error handling and logging in data extraction process; add support for saving unsuccessful profiles and debug information. Update .gitignore to include logs directory.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles.xlsx
+++ b/output/extracted_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,25 +507,29 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Debbie</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Gray</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
           <t>Director</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 310</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Contact via teams</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>dgray@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -534,29 +538,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/services/grant-and-project-development/our-people/soren-newman</t>
+          <t>https://www.uidaho.edu/cals/people/harpreet-kaur</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Soren</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Newman</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Grant &amp; Project Dev</t>
+          <t>Statistician</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>hkaur@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -565,29 +565,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/harpreet-kaur</t>
+          <t>https://www.uidaho.edu/cals/people/madison-mcguire</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Harpreet</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Kaur</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Statistician</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+          <t>Administrative Specialist</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 52 (Dean's Suite)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>208-885-6681</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>madisonmcguire@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
@@ -596,29 +600,29 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/madison-mcguire</t>
+          <t>https://www.uidaho.edu/cals/people/savanah-nunes</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Madison</t>
-        </is>
-      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>McGuire</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Administrative Specialist</t>
+          <t>Media and Communications Manager</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>208-539-7490</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>snunes@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -627,26 +631,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/savanah-nunes</t>
+          <t>https://www.uidaho.edu/cals/people/brandi-chastain</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Savanah</t>
-        </is>
-      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Nunes</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Media and Communications Manager</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
@@ -658,26 +650,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/steve-greene</t>
+          <t>https://www.uidaho.edu/cals/people/brian-kelly</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Steve</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Greene</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Program Manager</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
@@ -689,127 +669,38 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/amy-calabretta</t>
+          <t>https://www.uidaho.edu/cals/people/carly-schoepflin</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Amy</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Calabretta</t>
-        </is>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Interim Director of Communications &amp; Strategic Initiatives</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+          <t>Director of Communications &amp; Strategic Initiatives</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 58</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>208-885-4037</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>craska@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://www.uidaho.edu/cals/people/angela-harley</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Angela</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Harley</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>College of Agricultural &amp; Life Sciences</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>https://www.uidaho.edu/cals/people/ann-barrington</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Ann</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Barrington</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Senior Director of Development</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>https://www.uidaho.edu/cals/people/ashley-baker</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Ashley</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Baker</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Instructional Media Designer</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: streamline main.py and enhance logging and error handling
Refactor main.py to simplify orchestration by removing global logger and LangSmith client setup, and passing them as parameters where needed. Update the processing loop to conditionally apply tracing based on settings. Enhance error handling for URL loading and processing, ensuring proper logging throughout. Clean up resource management in cleanup.py to prevent double execution. Update uidaho_urls.json by removing outdated entries and adjust the refactoring plan in refactoring.md to reflect these changes.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles.xlsx
+++ b/output/extracted_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,29 +542,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/harpreet-kaur</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-harpreet-kaur.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=347fbb20f8d34085abb16563707b2cde</t>
-        </is>
-      </c>
+          <t>https://www.uidaho.edu/cals/services/grant-and-project-development/our-people/soren-newman</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Statistician</t>
+          <t>Grant &amp; Project Dev</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>hkaur@uidaho.edu</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -573,12 +565,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/madison-mcguire</t>
+          <t>https://www.uidaho.edu/cals/people/robyn-wakefield</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-madison-mcguire.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=cffce2fefade4171ae6a7fa8e3b9015c</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-robin-wakefield.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=d2529ad48aea4cccae4246b68ea2e9e3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -596,33 +588,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/savanah-nunes</t>
+          <t>https://www.uidaho.edu/cals/people/sharon-murdock</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-savanah-nunes.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=dfa96124f83244bb910bcdddfc069582</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-sharon-murdock.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=1c743421f1754058bf05b061c742eb01</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Media and Communications Manager</t>
-        </is>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>208-539-7490</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>snunes@uidaho.edu</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -631,12 +611,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/brandi-chastain</t>
+          <t>https://www.uidaho.edu/cals/people/stephanie-bunney</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-brandi-chastain.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=22142ccc9d92424bb2a8a749cfa522ff</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-stephanie-bunney.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=f80e978f7d8a453393d9ffcff1d9006d</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -654,12 +634,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/brian-kelly</t>
+          <t>https://www.uidaho.edu/cals/people/tammy-greenwalt</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-brian-kelly.jpg?h=300&amp;la=en&amp;w=300&amp;rev=7a40f27403394619b8297896d9959f5c</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-tammy-greenwalt.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=a23705edf2564c34ac09e376a552d5b8</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -677,26 +657,189 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/carly-schoepflin</t>
+          <t>https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/amanda-moore-kriwox</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-carly-schoepflin.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=b17fed7c84c84bd3bd657141bd56205f</t>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aelc/people/1200x1200-amanda-moore-kriwox.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=27d7a34316b14806af02663e3b97e24f</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Program Specialist, Academic Coordinator</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Room B-64</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>208-736-3624</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>akriwox@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/sarah-swenson</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aelc/people/1200x1200-sarah-swenson.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=504be8f9e88247bba3ffd72988b8ff84</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Administrative Coordinator</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ag Education, Room 101</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>208-885-6358</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>sswenson@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/alexander-maas</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-alexander-maas.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=19b14f042e724ed185c93ac5ba23ee4e</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/andres-trujillo-barrera</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-andres-trujillo-barrera.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=40e0a170ed544ec5a45f041448cd78f6</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Associate Professor &amp; Director, Agricultural Commodity Risk Management Program</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 37</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>208-885-1151</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>aatrujillo@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/brett-wilder</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-brett-wilder.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=99f0a4f8cd7b4eafac548c84d342b6d1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/brenda-murdoch</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-brenda-murdoch.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=ac4caf11e8b8495bbda2925b84bf85df</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: encapsulate application logic in ProfileExtractorApp class
Refactor main.py to encapsulate the profile extraction process within a new ProfileExtractorApp class. This change organizes state management and lifecycle handling, moving key functions into methods of the class. Enhance logging and error handling throughout the application, ensuring consistent behavior during execution. Update the main function to instantiate and run the new app class, improving modularity and maintainability of the codebase.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles.xlsx
+++ b/output/extracted_profiles.xlsx
@@ -707,26 +707,10 @@
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Administrative Coordinator</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Ag Education, Room 101</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>208-885-6358</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>sswenson@uidaho.edu</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -808,13 +792,33 @@
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Assistant Professor &amp; Area Extension Educator — Farm Business Management</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Room C1</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>208-885-0263</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>bwilder@uidaho.edu</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>['M.S., University of Idaho, 2019', 'B.S., University of Idaho, 2017']</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
chore: update profile extraction instructions in nodes.py and refresh output files
Revise the extraction instructions in nodes.py to provide clearer guidelines for extracting faculty profile information, ensuring adherence to the `ProfileData` JSON schema. Update the output files extracted_profiles.xlsx and extracted_profiles_errors.xlsx to reflect the latest changes in the extraction process.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles.xlsx
+++ b/output/extracted_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,9 +511,17 @@
           <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-debbie-gray.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=5cf7cf91a33849419def2bc4d4d030f3</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Debbie</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Gray</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Director</t>
@@ -524,20 +532,32 @@
           <t>Ag Science, Room 310</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Contact via teams</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>dgray@uidaho.edu</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Grant and Project Development</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -546,21 +566,53 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Soren</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Newman</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>Grant &amp; Project Dev</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>E. J. Iddings Agricultural Science Laboratory, Room 52 606 S Rayburn St</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>208-885-6681</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ag@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -573,17 +625,53 @@
           <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-robin-wakefield.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=d2529ad48aea4cccae4246b68ea2e9e3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Robyn</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Wakefield</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Grants Specialist</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 6</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>208-885-6322</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>rwakefield@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -596,17 +684,53 @@
           <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-sharon-murdock.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=1c743421f1754058bf05b061c742eb01</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sharon</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Murdock</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Student Services Manager</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 65</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>208-885-7984</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>sharonm@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -619,17 +743,57 @@
           <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-stephanie-bunney.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=f80e978f7d8a453393d9ffcff1d9006d</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Stephanie</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bunney</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Financial Specialist</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 40I</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>208-885-6346</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>stephanie@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Administrative Services</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -642,17 +806,57 @@
           <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-tammy-greenwalt.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=a23705edf2564c34ac09e376a552d5b8</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Tammy</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Greenwalt</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Financial Specialist</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 40J</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>208-885-6684</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>tammyg@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Administrative Services</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -665,9 +869,17 @@
           <t>/-/media/uidaho-responsive/images/cals/departments/aelc/people/1200x1200-amanda-moore-kriwox.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=27d7a34316b14806af02663e3b97e24f</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Amanda</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Moore-Kriwox</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Program Specialist, Academic Coordinator</t>
@@ -688,10 +900,26 @@
           <t>akriwox@uidaho.edu</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Education, Leadership and Communications</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>['Ph.D. candidate, University of Idaho', 'M.S., University of Idaho', 'B.S., University of Idaho', 'A.A., College of Southern Idaho']</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>['Distance Education']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -704,17 +932,57 @@
           <t>/-/media/uidaho-responsive/images/cals/departments/aelc/people/1200x1200-sarah-swenson.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=504be8f9e88247bba3ffd72988b8ff84</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Swenson</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Administrative Coordinator</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ag Education, Room 101</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>208-885-6358</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>sswenson@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Education, Leadership and Communications</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -727,122 +995,183 @@
           <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-alexander-maas.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=19b14f042e724ed185c93ac5ba23ee4e</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alexander</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Maas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 28B</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>208-885-5786</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>alexmaas@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>['Ph.D., Colorado State University', 'M.S., University of Connecticut', 'B.S., Boston University']</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>['allocation and valuation of scarce resources', 'water related issues', 'economic implications of resource management and local policies']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/andres-trujillo-barrera</t>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/brett-wilder</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-andres-trujillo-barrera.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=40e0a170ed544ec5a45f041448cd78f6</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-brett-wilder.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=99f0a4f8cd7b4eafac548c84d342b6d1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Brett</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Wilder</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Associate Professor &amp; Director, Agricultural Commodity Risk Management Program</t>
+          <t>Assistant Professor &amp; Area Extension Educator — Farm Business Management</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Ag Science, Room 37</t>
+          <t>Room C1</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>208-885-1151</t>
+          <t>208-885-0263</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>aatrujillo@uidaho.edu</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+          <t>bwilder@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>University of Idaho Extension</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>['M.S., University of Idaho, 2019', 'B.S., University of Idaho, 2017']</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>['Agricultural marketing', 'Commodity risk management', 'Agricultural finance']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/brett-wilder</t>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/brenda-murdoch</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-brett-wilder.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=99f0a4f8cd7b4eafac548c84d342b6d1</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
+          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-brenda-murdoch.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=ac4caf11e8b8495bbda2925b84bf85df</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Brenda</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Murdoch</t>
+        </is>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Assistant Professor &amp; Area Extension Educator — Farm Business Management</t>
+          <t>Professor</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Room C1</t>
+          <t>Ag Biotech, Room 311</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>208-885-0263</t>
+          <t>208-885-2088</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>bwilder@uidaho.edu</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+          <t>bmurdoch@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Department of Animal, Veterinary and Food Sciences</t>
+        </is>
+      </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>['M.S., University of Idaho, 2019', 'B.S., University of Idaho, 2017']</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/brenda-murdoch</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-brenda-murdoch.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=ac4caf11e8b8495bbda2925b84bf85df</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
+          <t>['Ph.D., University of Alberta', 'B.Sc., University of Alberta']</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>['BSE Cattle', 'Gene and quantitative trait mapping', 'Genetic improvement', 'Genome wide association studies', 'Genotyping', 'Infertility', 'Livestock genomics', 'Sheep', 'genetic testing in the Biotechnology lab', 'Livestock Genetics &amp; Phenotypic Trait Research', 'Study genetically mediated regulation of economically important traits in livestock species including; beef cattle, dairy cattle and sheep']</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: enhance profile data structure and extraction process
Add a new DegreeInfo model to structure academic degree information, including type, institution, and year. Update the ProfileData schema to reflect this change, allowing for a more detailed representation of faculty qualifications. Revise extraction instructions in nodes.py to clarify the expected format for degrees. Additionally, update uidaho_urls.json by adding new URLs and removing outdated entries, ensuring the data source remains current. Refresh output files to align with the latest extraction process.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles.xlsx
+++ b/output/extracted_profiles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,24 +582,12 @@
           <t>Grant &amp; Project Dev</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>E. J. Iddings Agricultural Science Laboratory, Room 52 606 S Rayburn St</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>208-885-6681</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>ag@uidaho.edu</t>
-        </is>
-      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Agricultural &amp; Life Sciences</t>
+          <t>College of Agricultural &amp; Life Sciences</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -617,54 +605,54 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/robyn-wakefield</t>
+          <t>https://www.uidaho.edu/cals/people/john-oconnell</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-robin-wakefield.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=d2529ad48aea4cccae4246b68ea2e9e3</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-john-oconnell.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=519806c40a2a4a848dbe3a6851f4371d</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Robyn</t>
+          <t>John</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Wakefield</t>
+          <t>O'Connell</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Grants Specialist</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Ag Science, Room 6</t>
-        </is>
-      </c>
+          <t>Assistant Director of Communications</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>208-885-6322</t>
+          <t>208-530-5959</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>rwakefield@uidaho.edu</t>
+          <t>joconnell@uidaho.edu</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>College of Agricultural and Life Sciences</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr"/>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Communications</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{'degree_type': 'B.S.', 'institution': 'University of Illinois', 'year': '2000'}]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -676,54 +664,58 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/sharon-murdock</t>
+          <t>https://www.uidaho.edu/cals/people/joseph-charles</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-sharon-murdock.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=1c743421f1754058bf05b061c742eb01</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-joseph-charles.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=d59ae349b5b4409982a34a0f503d006b</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sharon</t>
+          <t>Joseph</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Murdock</t>
+          <t>Charles</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Student Services Manager</t>
+          <t>Assistant Director of Budget, Finance &amp; Compliance</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Ag Science, Room 65</t>
+          <t>Ag Science, Room 40L</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>208-885-7984</t>
+          <t>208-885-7550</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>sharonm@uidaho.edu</t>
+          <t>jcharles@uidaho.edu</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>College of Agricultural &amp; Life Sciences</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr"/>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Administrative Services</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{'degree_type': 'M.S.', 'institution': 'University of Idaho', 'year': '2019'}, {'degree_type': 'B.S.', 'institution': 'University of Idaho', 'year': '2014'}]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -735,43 +727,35 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/stephanie-bunney</t>
+          <t>https://www.uidaho.edu/cals/people/julia-piaskowski</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-stephanie-bunney.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=f80e978f7d8a453393d9ffcff1d9006d</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-julia-piaskowski.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=150d0680b02d49e292803431bce5e767</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Julia</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bunney</t>
+          <t>Piaskowski</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Financial Specialist</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Ag Science, Room 40I</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>208-885-6346</t>
-        </is>
-      </c>
+          <t>Director of Statistical Programs</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>stephanie@uidaho.edu</t>
+          <t>jpiaskowski@uidaho.edu</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -781,7 +765,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Administrative Services</t>
+          <t>Statistical Programs</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -798,43 +782,39 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/tammy-greenwalt</t>
+          <t>https://www.uidaho.edu/cals/people/julie-colson</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-tammy-greenwalt.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=a23705edf2564c34ac09e376a552d5b8</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-julie-colson.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=745f743f8ce7417a987c68be1ac9853e</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tammy</t>
+          <t>Julie</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Greenwalt</t>
+          <t>Colson</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Financial Specialist</t>
+          <t>Grants and Research Associate</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Ag Science, Room 40J</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>208-885-6684</t>
-        </is>
-      </c>
+          <t>Ag Science, Room 310</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>tammyg@uidaho.edu</t>
+          <t>colson@uidaho.edu</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -844,7 +824,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Administrative Services</t>
+          <t>Grant and Project Development</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -861,116 +841,116 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/amanda-moore-kriwox</t>
+          <t>https://www.uidaho.edu/cals/people/kacie-hoffman</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/aelc/people/1200x1200-amanda-moore-kriwox.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=27d7a34316b14806af02663e3b97e24f</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-kacie-hoffman.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=4932459dbb664d0cadf002038951aa0c</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Kacie</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Moore-Kriwox</t>
+          <t>Hoffman</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Program Specialist, Academic Coordinator</t>
+          <t>Director of Recruitment and Student Engagement</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Room B-64</t>
+          <t>Ag Science, Room 65</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>208-736-3624</t>
+          <t>208-885-7984</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>akriwox@uidaho.edu</t>
+          <t>kacieh@uidaho.edu</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>College of Agricultural and Life Sciences</t>
+          <t>College of Agricultural &amp; Life Sciences</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Department of Agricultural Education, Leadership and Communications</t>
+          <t>Academic Programs</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>['Ph.D. candidate, University of Idaho', 'M.S., University of Idaho', 'B.S., University of Idaho', 'A.A., College of Southern Idaho']</t>
+          <t>[{'degree_type': 'M.S.', 'institution': 'University of Idaho', 'year': '2018'}, {'degree_type': 'B.S.', 'institution': 'University of Idaho', 'year': '2015'}]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>['Distance Education']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/sarah-swenson</t>
+          <t>https://www.uidaho.edu/cals/people/linda-wilson</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/aelc/people/1200x1200-sarah-swenson.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=504be8f9e88247bba3ffd72988b8ff84</t>
+          <t>/-/media/uidaho-responsive/images/default-placeholders/nophoto-versioned.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=065da4d6add54174bf85a968bfa99f92</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Swenson</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Administrative Coordinator</t>
+          <t>Financial Specialist</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Ag Education, Room 101</t>
+          <t>Ag Science, Room 40H</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>208-885-6358</t>
+          <t>208-885-8929</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>sswenson@uidaho.edu</t>
+          <t>lindawilson@uidaho.edu</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>College of Agricultural and Life Sciences</t>
+          <t>College of Agricultural &amp; Life Sciences</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Department of Agricultural Education, Leadership and Communications</t>
+          <t>Administrative Services</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -987,43 +967,43 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/alexander-maas</t>
+          <t>https://www.uidaho.edu/cals/people/lori-vermaas</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-alexander-maas.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=19b14f042e724ed185c93ac5ba23ee4e</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-lori-vermaas.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=0b5929fad45f4ba49fcbb6b0904a8deb</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Lori</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Maas</t>
+          <t>Vermaas</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Publishing Editor</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Ag Science, Room 28B</t>
+          <t>Ag Science, Room 10B</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>208-885-5786</t>
+          <t>208-885-1211</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>alexmaas@uidaho.edu</t>
+          <t>loriv@uidaho.edu</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1033,143 +1013,1379 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Department of Agricultural Economics and Rural Sociology</t>
+          <t>University of Idaho Extension Publishing</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>['Ph.D., Colorado State University', 'M.S., University of Connecticut', 'B.S., Boston University']</t>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'University of Iowa', 'year': '2000'}, {'degree_type': 'M.S.', 'institution': 'University of Iowa', 'year': '1992'}, {'degree_type': 'B.A.', 'institution': 'University of Texas-Austin', 'year': '1989'}]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>['allocation and valuation of scarce resources', 'water related issues', 'economic implications of resource management and local policies']</t>
+          <t>['Trees and plants', 'Natural history and its illustration in America (birds, trees, other plants)', 'American and European plant hunters, seventeenth through nineteenth centuries', 'American environmental history', 'American late nineteenth and early twentieth century cultural history', 'American visual culture, 1850-1950']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/brett-wilder</t>
+          <t>https://www.uidaho.edu/cals/people/lynna-stewart</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-brett-wilder.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=99f0a4f8cd7b4eafac548c84d342b6d1</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-lynna-stewert.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=81532d655e0543908e86b97724a6fff9</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Brett</t>
+          <t>Lynna</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Wilder</t>
+          <t>Stewart</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Assistant Professor &amp; Area Extension Educator — Farm Business Management</t>
+          <t>Graphic Designer</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Room C1</t>
+          <t>Ag Science, Room 6</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>208-885-0263</t>
+          <t>208-885-5120</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>bwilder@uidaho.edu</t>
+          <t>lynnas@uidaho.edu</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>University of Idaho Extension</t>
+          <t>College of Agricultural and Life Sciences</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Department of Agricultural Economics and Rural Sociology</t>
+          <t>Communications</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>['M.S., University of Idaho, 2019', 'B.S., University of Idaho, 2017']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>['Agricultural marketing', 'Commodity risk management', 'Agricultural finance']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/brenda-murdoch</t>
+          <t>https://www.uidaho.edu/cals/people/margarita-cardona</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-brenda-murdoch.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=ac4caf11e8b8495bbda2925b84bf85df</t>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-margarita-cardona.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=6e3e65acd8fa462ab34cd83916e53110</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>Margarita</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Murdoch</t>
+          <t>Cardona</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>Chief Business Officer</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>U of I Boise, Suite 120L</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>208-364-4687</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>mcardona@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Administrative Services</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'CMA', 'institution': None, 'year': '2014'}, {'degree_type': 'M.S.', 'institution': 'Universidad de los Andes, Bogota, Colombia', 'year': '2003'}, {'degree_type': 'B.S.', 'institution': 'Universidad del Norte, Barranquilla, Colombia', 'year': '2001'}]</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/mark-corrao</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-mark-corrao.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=f847a073e4274ca1a66345999057d9af</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Corrao</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Adjunct Faculty</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>208-310-6732</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>mcorrao@nmi2.com</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'University of Idaho', 'year': '2015'}, {'degree_type': 'M.S.', 'institution': 'Colorado State University', 'year': '2007'}, {'degree_type': 'B.S.', 'institution': 'University of Idaho', 'year': '2004'}]</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/matt-doumit</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-matt-doumit.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=5cba8660e577438fb310b4452342dbd4</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Matt</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>E.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Doumit</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Senior Associate Dean &amp; Director, Academic Programs</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 65</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>208-885-7984</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>mdoumit@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Academic Programs</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Michigan State University, East Lansing', 'year': '1994'}, {'degree_type': 'M.S.', 'institution': 'South Dakota State University', 'year': '1989'}, {'degree_type': 'B.S.', 'institution': 'Washington State University', 'year': '1987'}]</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>['Beef quality', 'Improve beef palatability']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/melinda-stafford</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-melinda-stafford.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=16677175f3074079b846e1dd5c4a8de1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Melinda</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Jean</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Stafford</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Director of Development</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Boise, Room 280A</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>208-364-4617</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>melindas@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>CALS Development</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'B.S.', 'institution': 'University of Idaho', 'year': '2011'}, {'degree_type': 'M.Ed.', 'institution': 'University of Georgia', 'year': '2013'}]</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/michael-parrella</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-michael-parrella.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=125776750b3f4f53b579fb698477d5a3</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>P.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Parrella</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Dean, College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 52</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>208-885-6681</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>mpp@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Virginia Polytechnic Institute and State University', 'year': '1980'}, {'degree_type': 'M.S.', 'institution': 'Virginia Polytechnic Institute and State University', 'year': '1977'}, {'degree_type': 'B.S.', 'institution': 'Rutgers-State University of Cook College', 'year': '1974'}]</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/nicole-wright</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-nicole-wright.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=2f1f0b7e8ba241bcac4d9f0835262d23</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Nicole</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Wright</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Assistant to Associate Deans/Directors for Extension &amp; Research</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 45</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>208-885-5883</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>nicolew@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>University of Idaho Extension</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'M.S.', 'institution': 'University of Idaho', 'year': '2022'}, {'degree_type': 'B.S.', 'institution': 'Lewis-Clark State College', 'year': '2011'}]</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/robert-haggerty</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-bob-haggerty.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=4ba56059cfd84111b03bd4d6d8d2ab1f</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Haggerty</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Director of International Programs</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 42</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>208-885-6681</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>haggerty@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/robyn-wakefield</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-robin-wakefield.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=d2529ad48aea4cccae4246b68ea2e9e3</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Robyn</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Wakefield</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Grants Specialist</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 6</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>208-885-6322</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>rwakefield@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/sharon-murdock</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-sharon-murdock.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=1c743421f1754058bf05b061c742eb01</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sharon</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Murdock</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Student Services Manager</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 65</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>208-885-7984</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>sharonm@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/stephanie-bunney</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-stephanie-bunney.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=f80e978f7d8a453393d9ffcff1d9006d</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Stephanie</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Bunney</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Financial Specialist</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 40I</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>208-885-6346</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>stephanie@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>College of Agricultural &amp; Life Sciences</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Administrative Services</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/people/tammy-greenwalt</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/college/our-people/1200x1200-tammy-greenwalt.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=a23705edf2564c34ac09e376a552d5b8</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Tammy</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Greenwalt</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Financial Specialist</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 40J</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>208-885-6684</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>tammyg@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Administrative Services</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/lorie-higgins</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-lorie-higgins.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=551465b4a749480ca12d5185ed22a958</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Lorie</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Higgins</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Professor &amp; Extension Specialist</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 24</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>208-669-1480</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>higgins@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Washington State University', 'year': '2001'}, {'degree_type': 'M.A.', 'institution': 'Washington State University', 'year': '1993'}, {'degree_type': 'B.A.', 'institution': 'University of Montana', 'year': '1989'}]</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>['Community-based decision-making', 'Asset-based visioning and action planning', 'Situation assessment', 'Collaborative processes', 'Strategic planning', 'Qualitative and participatory research methods', 'Regional cultural industries initiatives', 'Community leadership development', 'Entrepreneurship', 'Ripple effects mapping evaluation']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/madison-griffin</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-madison-griffin.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=95b63e5323c9453394e80a2bebebd236</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Madison</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Griffin</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Administrative Specialist &amp; Academic Advisor</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 39</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>208-885-6264</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>mgriffin@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'M.A.', 'institution': 'University of Idaho', 'year': '2014'}]</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/norm-ruhoff</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-norm-ruhoff.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=124ecd9b49ba49a893b442357087f564</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Norm</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Ruhoff</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Clinical Associate Professor</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 39B</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>208-885-1707</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>nruhoff@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'M.S.', 'institution': 'University of Idaho', 'year': '1988'}, {'degree_type': 'B.S.', 'institution': 'University of Idaho', 'year': '1983'}]</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/patrick-hatzenbuehler</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-patrick-hatzenbuehler.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=6a147ad5beb54100af27dcb2c0966381</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Patrick</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Hatzenbuehler</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Associate Professor &amp; Extension Specialist</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Room 63</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>208-736-3607</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>phatzenbuehler@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Purdue University', 'year': '2016'}, {'degree_type': 'M.S.', 'institution': 'Louisiana State University', 'year': '2010'}, {'degree_type': 'A.B.', 'institution': 'Georgetown University', 'year': '2006'}]</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>['Agricultural commodity market supply and demand fundamentals', 'Agricultural commodity price analysis', 'Agricultural development', 'Agricultural policy']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/philip-watson</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-philip-watson.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=fc45bca76dda4d74b2eb33d67e4f5e87</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Philip</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Watson</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>Professor</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Ag Biotech, Room 311</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>208-885-2088</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>bmurdoch@uidaho.edu</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 30</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>208-962-1312</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>pwatson@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
         <is>
           <t>College of Agricultural and Life Sciences</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Colorado State University', 'year': '2006'}, {'degree_type': 'M.Ag.', 'institution': 'Colorado State University', 'year': '2003'}, {'degree_type': 'B.S.', 'institution': 'Taylor University', 'year': '1998'}]</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>['natural resource and regional development economics', 'role of natural resources in the economic health of communities', 'evidence based economic development planning']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/xiaoli-etienne</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-xiaoli-etienne.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=806baa93508242f9aab489177c19b3b9</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Xiaoli</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Etienne</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Professor &amp; Idaho Wheat Commission Endowed Chair in Commodity Risk Management</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 25</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>208-885-0133</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>xetienne@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'University of Illinois at Urbana Champaign', 'year': '2013'}, {'degree_type': 'M.S.', 'institution': 'University of Illinois at Urbana Champaign', 'year': '2009'}, {'degree_type': 'B.A.', 'institution': 'Renmin University of China', 'year': '2007'}]</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/xiaoxue-du</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/aers/people/1200x1200-xiaoxue-rita-du.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=bd3084f9779c493886540fbb9b37d80d</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Xiaoxue</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Du</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 39D</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>208-885-4277</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>xiaoxuedu@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Department of Agricultural Economics and Rural Sociology</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'University of California, Berkeley', 'year': '2017'}, {'degree_type': 'M.S.', 'institution': 'University of Idaho', 'year': '2012'}, {'degree_type': 'B.M.', 'institution': 'Tianjin Institute of Urban Construction', 'year': '2006'}]</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>['Crop insurance and contracts', 'Applied risk analysis', 'International trade']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/amin-ahmadzadeh</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-amin-ahmadzadeh.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=8319d0916f98491aa88c2a910a91f736</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Amin</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Ahmadzadeh</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ag Science, Room 219</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>208-885-7409</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>amin@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>Department of Animal, Veterinary and Food Sciences</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>['Ph.D., University of Alberta', 'B.Sc., University of Alberta']</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>['BSE Cattle', 'Gene and quantitative trait mapping', 'Genetic improvement', 'Genome wide association studies', 'Genotyping', 'Infertility', 'Livestock genomics', 'Sheep', 'genetic testing in the Biotechnology lab', 'Livestock Genetics &amp; Phenotypic Trait Research', 'Study genetically mediated regulation of economically important traits in livestock species including; beef cattle, dairy cattle and sheep']</t>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Virginia Tech', 'year': None}, {'degree_type': 'M.S.', 'institution': 'Virginia Tech', 'year': None}, {'degree_type': 'B.S.', 'institution': 'Delaware Valley', 'year': None}]</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>['Applied cattle reproduction, with an emphasis on fertility and management', 'Develop a systematic breeding program for dairy cattle to increase fertility rates and improve reproductive and economic advantages of artificial insemination (AI) on dairy farms', 'Investigate the role of environment, management and diseases on cattle reproduction', 'Interaction between nutrition and reproduction', 'Enhancing conception rate by reducing early embryonic loss', 'Collaborate with UI dairy extension specialist Joe Dalton and reproductive physiologist Tracy Davis to address issues on farms, specifically the direct implications on practical reproductive management']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/amy-skibiel</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-amy-skibiel.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=9399fa6d0e53427dbc9d9433d2722705</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Skibiel</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Associate Professor — Lactation Physiology</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ag Biotech, Room 303</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>208-885-1161</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>askibiel@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Department of Animal, Veterinary and Food Sciences</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Auburn University', 'year': '2012'}, {'degree_type': 'M.S.', 'institution': 'Auburn University', 'year': '2007'}, {'degree_type': 'B.S.', 'institution': 'Juniata College', 'year': '2003'}]</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>['Impacts of the environment and management practices on mammary gland physiology and milk production', 'Association between postnatal physiology and performance and the fetal growth environment', 'How offspring development and health is shaped by the nutritive and bioactive components in mother’s milk']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/benton-glaze</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>/-/media/uidaho-responsive/images/cals/departments/avfs/people/1200x1200-benton-glaze.jpg?h=1200&amp;la=en&amp;w=1200&amp;rev=9a6661856c3c41be8ee2ae83d0948892</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Benton</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Glaze</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Professor &amp; Extension Specialist — Beef</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>208-736-3638</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>bglaze@uidaho.edu</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>College of Agricultural and Life Sciences</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Department of Animal, Veterinary and Food Sciences</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>[{'degree_type': 'Ph.D.', 'institution': 'Kansas State University', 'year': None}, {'degree_type': 'M.S.', 'institution': 'University of Missouri-Columbia', 'year': None}, {'degree_type': 'B.S.', 'institution': 'Tarleton State University', 'year': None}]</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>['breeding and genetics', 'beef quality assurance', 'general management', 'reproduction']</t>
         </is>
       </c>
     </row>

</xml_diff>